<commit_message>
Built site for MassWateR: 1.0.0.9000@bb1cc0b
</commit_message>
<xml_diff>
--- a/ExampleWQX.xlsx
+++ b/ExampleWQX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289AF66D-5555-4C9D-BA9D-6AD072E59E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C350E7-D3B3-4754-8AA1-9345041D9BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29820" yWindow="2580" windowWidth="22710" windowHeight="11295" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
+    <workbookView xWindow="35520" yWindow="4035" windowWidth="18165" windowHeight="9030" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>APHA</t>
   </si>
   <si>
-    <t>MassWateR</t>
-  </si>
-  <si>
     <t>EPA 1603</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>Filtered, Lab</t>
+  </si>
+  <si>
+    <t>MassBays</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,10 +521,10 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -578,13 +578,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>9</v>
@@ -595,16 +595,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>9</v>
@@ -618,19 +618,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Built site for MassWateR: 1.0.0.9000@16a249f
</commit_message>
<xml_diff>
--- a/ExampleWQX.xlsx
+++ b/ExampleWQX.xlsx
@@ -1,40 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Example input files\Official Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C350E7-D3B3-4754-8AA1-9345041D9BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8085BA-692E-46C5-AB6F-BEB1B5FA209D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35520" yWindow="4035" windowWidth="18165" windowHeight="9030" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
   <si>
     <t>Parameter</t>
   </si>
@@ -54,6 +46,24 @@
     <t>E.coli</t>
   </si>
   <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Available Values</t>
+  </si>
+  <si>
+    <t>see parameter list</t>
+  </si>
+  <si>
+    <t>All cells in the matrix must either have a value or "na".</t>
+  </si>
+  <si>
     <t>Analytical Method</t>
   </si>
   <si>
@@ -69,12 +79,18 @@
     <t>APHA</t>
   </si>
   <si>
-    <t>EPA 1603</t>
+    <t>MassWateR</t>
   </si>
   <si>
     <t>USEPA</t>
   </si>
   <si>
+    <t>defined in WQX by organization</t>
+  </si>
+  <si>
+    <t>standard list in WQX</t>
+  </si>
+  <si>
     <t>Method Speciation</t>
   </si>
   <si>
@@ -87,20 +103,70 @@
     <t>Unfiltered</t>
   </si>
   <si>
-    <t>TDP</t>
-  </si>
-  <si>
-    <t>Filtered, Lab</t>
-  </si>
-  <si>
-    <t>MassBays</t>
+    <t>The Meta tab must be formatted exactly like the Meta template, with all of the following fields.</t>
+  </si>
+  <si>
+    <t>The Meta tab must be the first tab in this workbook.</t>
+  </si>
+  <si>
+    <t>Enter the Result Sample Fraction for this parameter.  Text name of fraction of sample associated with result, required for certain characteristics.  Not applicable for field measurements/observations.</t>
+  </si>
+  <si>
+    <t>Enter the Method Speciation for this parameter.  Identifies the chemical speciation in which the measured result is expressed.  Not applicable for field measurements/observations.</t>
+  </si>
+  <si>
+    <t>Enter the Analytical Method ID for this parameter.  ID number assigned by method publisher.  Not applicable for field measurements/observations.</t>
+  </si>
+  <si>
+    <t>Enter the Context for the Analytical Method ID.  Source of method.  Not applicable for field measurements/observations.</t>
+  </si>
+  <si>
+    <t>Name of the measured parameter.
+- Note that this can be either the WQX or Simple parameter name.  However, if a parameter is distinguished by Sample Fraction only (i.e. TDP, TDN), then the Simple parameter name must be used here and in all other files (Results, DQO, etc.)</t>
+  </si>
+  <si>
+    <t>standard list in WQX
+Recommended:  Filtered, lab; Filtered, field; Unfiltered; Non-Filterable (Particle)</t>
+  </si>
+  <si>
+    <t>Enter the Context for the Sampling Method IDs that are used for sampling this parameter.  Not applicable for field measurements/observations.  If you are using the standard methods defined by MassWateR, enter the context "MassWateR".</t>
+  </si>
+  <si>
+    <t>Water Temp</t>
+  </si>
+  <si>
+    <t>Sp Conductance</t>
+  </si>
+  <si>
+    <t>200.7</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>as N</t>
+  </si>
+  <si>
+    <t>300.0</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>4500-NH3 D</t>
+  </si>
+  <si>
+    <t>COLILERT</t>
+  </si>
+  <si>
+    <t>IDEXX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +182,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -125,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -163,26 +245,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,142 +615,342 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973C1027-43ED-409D-9786-38F45BEFD8D3}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="6" customWidth="1"/>
-    <col min="2" max="6" width="13.109375" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="6"/>
+    <col min="1" max="1" width="15.81640625" style="14" customWidth="1"/>
+    <col min="2" max="6" width="13.1796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="11" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.26953125" customWidth="1"/>
+    <col min="2" max="2" width="96.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="D11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>